<commit_message>
Added new Quastions in the SIQ sheet Signed-off-by: mayabdelsalam <mayabdalsalam777@gmail.com>
</commit_message>
<xml_diff>
--- a/Input documents/SIQ.xlsx
+++ b/Input documents/SIQ.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -20,74 +19,74 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
-  <si>
-    <t xml:space="preserve">Req ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Asked By</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SIQ ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Question</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proposed Answer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Expected Return Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Return Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Answer</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
+  <si>
+    <t>Req ID</t>
+  </si>
+  <si>
+    <t>Asked By</t>
+  </si>
+  <si>
+    <t>SIQ ID</t>
+  </si>
+  <si>
+    <t>Question</t>
+  </si>
+  <si>
+    <t>Proposed Answer</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Expected Return Date</t>
+  </si>
+  <si>
+    <t>Return Date</t>
+  </si>
+  <si>
+    <t>Answer</t>
   </si>
   <si>
     <t xml:space="preserve">Req_PO1_DGC_CYRS_005_v1.0 </t>
   </si>
   <si>
-    <t xml:space="preserve">May Abdelsalam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SIQ_PO1_DGC_CYRS_001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What will happen when the user enters an operaion
+    <t>May Abdelsalam</t>
+  </si>
+  <si>
+    <t>SIQ_PO1_DGC_CYRS_001</t>
+  </si>
+  <si>
+    <t>What will happen when the user enters an operaion
 while one is already displayed</t>
   </si>
   <si>
-    <t xml:space="preserve">The new operaion will be denied</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21/1/2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22/1/2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">31/1/2020</t>
+    <t>The new operaion will be denied</t>
+  </si>
+  <si>
+    <t>21/1/2020</t>
+  </si>
+  <si>
+    <t>22/1/2020</t>
+  </si>
+  <si>
+    <t>31/1/2020</t>
   </si>
   <si>
     <t xml:space="preserve">The new operation will be applied and 
 The old one will be denied. </t>
   </si>
   <si>
-    <t xml:space="preserve">Req_PO1_DGC_CYRS_008_v1.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SIQ_PO1_DGC_CYRS_002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shall the system have an ON/OFF button? If yes what will the type of this button and how will it enteract with the system</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A Tactile switch that  if pressed once it opens the calculator and if pressed twice it shuts it off</t>
+    <t>Req_PO1_DGC_CYRS_008_v1.0</t>
+  </si>
+  <si>
+    <t>SIQ_PO1_DGC_CYRS_002</t>
+  </si>
+  <si>
+    <t>Shall the system have an ON/OFF button? If yes what will the type of this button and how will it enteract with the system</t>
+  </si>
+  <si>
+    <t>A Tactile switch that  if pressed once it opens the calculator and if pressed twice it shuts it off</t>
   </si>
   <si>
     <r>
@@ -95,7 +94,6 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
-        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Yes, the system should have an ON/OFF button and it’s fine to be a tactile switch and will interact with the system as follows: if </t>
@@ -105,34 +103,33 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
-        <family val="0"/>
       </rPr>
-      <t xml:space="preserve">pressed once it switches on and if pressed twice it switches off.</t>
+      <t>pressed once it switches on and if pressed twice it switches off.</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Req_PO1_DGC_CYRS_009_v1.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SIQ_PO1_DGC_CYRS_003</t>
+    <t>Req_PO1_DGC_CYRS_009_v1.0</t>
+  </si>
+  <si>
+    <t>SIQ_PO1_DGC_CYRS_003</t>
   </si>
   <si>
     <t xml:space="preserve">Should the calculator handel negative numbers? </t>
   </si>
   <si>
-    <t xml:space="preserve">It should</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes,it should handle any negative numbers or results.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Req_PO1_DGC_CYRS_010_v1.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SIQ_PO1_DGC_CYRS_004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">should the system handel division by zero? If it should what will be the message displayed for the user?</t>
+    <t>It should</t>
+  </si>
+  <si>
+    <t>Yes,it should handle any negative numbers or results.</t>
+  </si>
+  <si>
+    <t>Req_PO1_DGC_CYRS_010_v1.0</t>
+  </si>
+  <si>
+    <t>SIQ_PO1_DGC_CYRS_004</t>
+  </si>
+  <si>
+    <t>should the system handel division by zero? If it should what will be the message displayed for the user?</t>
   </si>
   <si>
     <r>
@@ -140,7 +137,6 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
-        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Yes, it should handle division by zero and the </t>
@@ -150,16 +146,14 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
-        <family val="0"/>
       </rPr>
-      <t xml:space="preserve">error</t>
+      <t>error</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
-        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> message will be appeared 
@@ -167,67 +161,80 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Req_PO1_DGC_CYRS_011_v1.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SIQ_PO1_DGC_CYRS_005</t>
-  </si>
-  <si>
-    <t xml:space="preserve">should the system handel floating numbers?</t>
+    <t>Req_PO1_DGC_CYRS_011_v1.0</t>
+  </si>
+  <si>
+    <t>SIQ_PO1_DGC_CYRS_005</t>
+  </si>
+  <si>
+    <t>should the system handel floating numbers?</t>
   </si>
   <si>
     <t xml:space="preserve">Yes, it should handle any fractions with a precision two numbers after floating point. </t>
+  </si>
+  <si>
+    <t>SIQ_PO1_DGC_CYRS_006</t>
+  </si>
+  <si>
+    <t>SIQ_PO1_DGC_CYRS_007</t>
+  </si>
+  <si>
+    <t>SIQ_PO1_DGC_CYRS_008</t>
+  </si>
+  <si>
+    <t>should be any key on the keypad that is corresponding to the negative sign or should the subtraction operation key be also a negative sign?</t>
+  </si>
+  <si>
+    <t>the negative operation key should be used as the negative sign of a number too.</t>
+  </si>
+  <si>
+    <t>if the user enters an operation at first before a number is entered, how should the system reacte?</t>
+  </si>
+  <si>
+    <t>it should not allow it if it is multiplication or division but shouldallow it if it is addition or subtraction as it should mean a sign in such case.</t>
+  </si>
+  <si>
+    <t>after performing an operation and displaying the resulte, what should be the behaviour of the system?</t>
+  </si>
+  <si>
+    <t>Req_PO1_DGC_CYRS_004_v1.0</t>
+  </si>
+  <si>
+    <t>Req_PO1_DGC_CYRS_012_v1.0</t>
+  </si>
+  <si>
+    <t>Req_PO1_DGC_CYRS_013_v1.0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="[$-409]M/D/YYYY"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-409]m/d/yyyy"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Cambria"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="3">
@@ -245,84 +252,57 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="8">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-  </cellStyleXfs>
-  <cellXfs count="7">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -381,36 +361,331 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="37.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="46.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="32.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="34.89"/>
+    <col min="1" max="1" width="37.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="3" max="3" width="22" customWidth="1"/>
+    <col min="4" max="4" width="46.33203125" customWidth="1"/>
+    <col min="5" max="5" width="32.33203125" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
+    <col min="7" max="7" width="19.6640625" customWidth="1"/>
+    <col min="8" max="8" width="16.109375" customWidth="1"/>
+    <col min="9" max="9" width="34.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -439,7 +714,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:9" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -468,7 +743,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="73.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:9" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>18</v>
       </c>
@@ -484,20 +759,20 @@
       <c r="E3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="6" t="n">
+      <c r="F3" s="6">
         <v>43832</v>
       </c>
-      <c r="G3" s="6" t="n">
+      <c r="G3" s="6">
         <v>43863</v>
       </c>
-      <c r="H3" s="6" t="n">
+      <c r="H3" s="6">
         <v>43863</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="25.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:9" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>23</v>
       </c>
@@ -513,20 +788,20 @@
       <c r="E4" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="6" t="n">
+      <c r="F4" s="6">
         <v>43832</v>
       </c>
-      <c r="G4" s="6" t="n">
+      <c r="G4" s="6">
         <v>43863</v>
       </c>
-      <c r="H4" s="6" t="n">
+      <c r="H4" s="6">
         <v>43863</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="37.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>28</v>
       </c>
@@ -542,20 +817,20 @@
       <c r="E5" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="6" t="n">
+      <c r="F5" s="6">
         <v>43832</v>
       </c>
-      <c r="G5" s="6" t="n">
+      <c r="G5" s="6">
         <v>43863</v>
       </c>
-      <c r="H5" s="6" t="n">
+      <c r="H5" s="6">
         <v>43863</v>
       </c>
       <c r="I5" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:9" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>32</v>
       </c>
@@ -569,64 +844,104 @@
         <v>34</v>
       </c>
       <c r="E6" s="5"/>
-      <c r="F6" s="6" t="n">
+      <c r="F6" s="6">
         <v>43832</v>
       </c>
-      <c r="G6" s="6" t="n">
+      <c r="G6" s="6">
         <v>43863</v>
       </c>
-      <c r="H6" s="6" t="n">
+      <c r="H6" s="6">
         <v>43863</v>
       </c>
       <c r="I6" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
+    <row r="7" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="7">
+        <v>43923</v>
+      </c>
+      <c r="G7" s="7">
+        <v>43923</v>
+      </c>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
+    <row r="8" spans="1:9" ht="69" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="7">
+        <v>43923</v>
+      </c>
+      <c r="G8" s="7">
+        <v>43923</v>
+      </c>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
+    <row r="9" spans="1:9" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>43</v>
+      </c>
       <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
+      <c r="F9" s="7">
+        <v>43923</v>
+      </c>
+      <c r="G9" s="7">
+        <v>43923</v>
+      </c>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
+      <c r="F10" s="7"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -637,7 +952,7 @@
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -648,7 +963,7 @@
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -659,7 +974,7 @@
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -670,7 +985,7 @@
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -681,7 +996,7 @@
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -693,12 +1008,7 @@
       <c r="I16" s="5"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Answering the new questions in SIQ sheet Signed-off-by: MMohamedAli74 <mmohamedali74@gmail.com>
</commit_message>
<xml_diff>
--- a/Input documents/SIQ.xlsx
+++ b/Input documents/SIQ.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="124519" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="49">
   <si>
     <t>Req ID</t>
   </si>
@@ -205,15 +205,21 @@
   <si>
     <t>Req_PO1_DGC_CYRS_013_v1.0</t>
   </si>
+  <si>
+    <t>If no new operation is required for 10s calculator shall be OFF</t>
+  </si>
+  <si>
+    <t>In case of "/ , * and +" a message shall be appear "Please enter an operand first". And in case of "-" it's OK</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]m/d/yyyy"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -278,7 +284,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -296,6 +302,12 @@
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -454,7 +466,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -489,7 +500,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -665,27 +675,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="37.6640625" customWidth="1"/>
+    <col min="1" max="1" width="37.7109375" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="46.33203125" customWidth="1"/>
-    <col min="5" max="5" width="32.33203125" customWidth="1"/>
+    <col min="4" max="4" width="46.28515625" customWidth="1"/>
+    <col min="5" max="5" width="32.28515625" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="19.6640625" customWidth="1"/>
-    <col min="8" max="8" width="16.109375" customWidth="1"/>
-    <col min="9" max="9" width="34.88671875" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" customWidth="1"/>
+    <col min="9" max="9" width="34.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="14.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -714,7 +724,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="42.75">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -743,7 +753,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="82.8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="85.5">
       <c r="A3" s="2" t="s">
         <v>18</v>
       </c>
@@ -772,7 +782,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="28.5">
       <c r="A4" s="5" t="s">
         <v>23</v>
       </c>
@@ -801,7 +811,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="57">
       <c r="A5" s="5" t="s">
         <v>28</v>
       </c>
@@ -830,7 +840,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="42.75">
       <c r="A6" s="5" t="s">
         <v>32</v>
       </c>
@@ -857,7 +867,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="57">
       <c r="A7" s="5" t="s">
         <v>45</v>
       </c>
@@ -876,13 +886,17 @@
       <c r="F7" s="7">
         <v>43923</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="9">
         <v>43923</v>
       </c>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-    </row>
-    <row r="8" spans="1:9" ht="69" x14ac:dyDescent="0.25">
+      <c r="H7" s="9">
+        <v>43925</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="71.25">
       <c r="A8" s="5" t="s">
         <v>44</v>
       </c>
@@ -901,13 +915,17 @@
       <c r="F8" s="7">
         <v>43923</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="9">
         <v>43923</v>
       </c>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-    </row>
-    <row r="9" spans="1:9" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="H8" s="9">
+        <v>43925</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="42.75">
       <c r="A9" s="5" t="s">
         <v>46</v>
       </c>
@@ -924,13 +942,17 @@
       <c r="F9" s="7">
         <v>43923</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="9">
         <v>43923</v>
       </c>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-    </row>
-    <row r="10" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="H9" s="9">
+        <v>43925</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="14.25">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -941,7 +963,7 @@
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
     </row>
-    <row r="11" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="14.25">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -952,7 +974,7 @@
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
     </row>
-    <row r="12" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="14.25">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -963,7 +985,7 @@
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
     </row>
-    <row r="13" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="14.25">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -974,7 +996,7 @@
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
     </row>
-    <row r="14" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="14.25">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -985,7 +1007,7 @@
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
     </row>
-    <row r="15" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="14.25">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -996,7 +1018,7 @@
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
     </row>
-    <row r="16" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="14.25">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>

</xml_diff>

<commit_message>
new updates to the CYRS document after viewing the SIQ sheet Signed-off-by: mayabdelsalam <mayabdalsalam777@gmail.com>
</commit_message>
<xml_diff>
--- a/Input documents/SIQ.xlsx
+++ b/Input documents/SIQ.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" iterateDelta="1E-4"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
   <si>
     <t>Req ID</t>
   </si>
@@ -205,21 +205,15 @@
   <si>
     <t>Req_PO1_DGC_CYRS_013_v1.0</t>
   </si>
-  <si>
-    <t>If no new operation is required for 10s calculator shall be OFF</t>
-  </si>
-  <si>
-    <t>In case of "/ , * and +" a message shall be appear "Please enter an operand first". And in case of "-" it's OK</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]m/d/yyyy"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -284,7 +278,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -302,12 +296,6 @@
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -466,6 +454,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -500,6 +489,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -675,27 +665,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.7109375" customWidth="1"/>
+    <col min="1" max="1" width="37.6640625" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="46.28515625" customWidth="1"/>
-    <col min="5" max="5" width="32.28515625" customWidth="1"/>
+    <col min="4" max="4" width="46.33203125" customWidth="1"/>
+    <col min="5" max="5" width="32.33203125" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="19.7109375" customWidth="1"/>
-    <col min="8" max="8" width="16.140625" customWidth="1"/>
-    <col min="9" max="9" width="34.85546875" customWidth="1"/>
+    <col min="7" max="7" width="19.6640625" customWidth="1"/>
+    <col min="8" max="8" width="16.109375" customWidth="1"/>
+    <col min="9" max="9" width="34.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14.25">
+    <row r="1" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -724,7 +714,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="42.75">
+    <row r="2" spans="1:9" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -753,7 +743,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="85.5">
+    <row r="3" spans="1:9" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>18</v>
       </c>
@@ -782,7 +772,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="28.5">
+    <row r="4" spans="1:9" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>23</v>
       </c>
@@ -811,7 +801,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="57">
+    <row r="5" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>28</v>
       </c>
@@ -840,7 +830,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="42.75">
+    <row r="6" spans="1:9" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>32</v>
       </c>
@@ -867,7 +857,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="57">
+    <row r="7" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>45</v>
       </c>
@@ -886,17 +876,13 @@
       <c r="F7" s="7">
         <v>43923</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="7">
         <v>43923</v>
       </c>
-      <c r="H7" s="9">
-        <v>43925</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="71.25">
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+    </row>
+    <row r="8" spans="1:9" ht="69" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>44</v>
       </c>
@@ -915,17 +901,13 @@
       <c r="F8" s="7">
         <v>43923</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="7">
         <v>43923</v>
       </c>
-      <c r="H8" s="9">
-        <v>43925</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="42.75">
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+    </row>
+    <row r="9" spans="1:9" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>46</v>
       </c>
@@ -942,17 +924,13 @@
       <c r="F9" s="7">
         <v>43923</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="7">
         <v>43923</v>
       </c>
-      <c r="H9" s="9">
-        <v>43925</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="14.25">
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+    </row>
+    <row r="10" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -963,7 +941,7 @@
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
     </row>
-    <row r="11" spans="1:9" ht="14.25">
+    <row r="11" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -974,7 +952,7 @@
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
     </row>
-    <row r="12" spans="1:9" ht="14.25">
+    <row r="12" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -985,7 +963,7 @@
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
     </row>
-    <row r="13" spans="1:9" ht="14.25">
+    <row r="13" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -996,7 +974,7 @@
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
     </row>
-    <row r="14" spans="1:9" ht="14.25">
+    <row r="14" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -1007,7 +985,7 @@
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
     </row>
-    <row r="15" spans="1:9" ht="14.25">
+    <row r="15" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -1018,7 +996,7 @@
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
     </row>
-    <row r="16" spans="1:9" ht="14.25">
+    <row r="16" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>

</xml_diff>

<commit_message>
Added new questions in the SIQ sheet
</commit_message>
<xml_diff>
--- a/Input documents/SIQ.xlsx
+++ b/Input documents/SIQ.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\mina\embeded_systems\ES_ITI_intake_40\Software_engineering\Calculator_repo\Software-Engineering\SWE_Calculator\Input documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500"/>
+    <workbookView xWindow="945" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="53">
   <si>
     <t>Req ID</t>
   </si>
@@ -205,6 +210,49 @@
   <si>
     <t>Req_PO1_DGC_CYRS_013_v1.0</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Req_PO1_DGC_CYRS_011_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>v1.0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Mina Yousry</t>
+  </si>
+  <si>
+    <t>SIQ_PO1_DGC_CYRS_009</t>
+  </si>
+  <si>
+    <t>7-2-2020</t>
+  </si>
+  <si>
+    <t>8-2-2020</t>
+  </si>
+  <si>
+    <t>if the operation is multiplication for example and the user entered negative sign should the system overwrite the operation or the second operand will be negative signed  ?</t>
+  </si>
 </sst>
 </file>
 
@@ -213,7 +261,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]m/d/yyyy"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -235,6 +283,29 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -278,7 +349,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -295,6 +366,13 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -375,6 +453,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -422,7 +503,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -457,7 +538,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -668,24 +749,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="37.6640625" customWidth="1"/>
+    <col min="1" max="1" width="37.7109375" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="46.33203125" customWidth="1"/>
-    <col min="5" max="5" width="32.33203125" customWidth="1"/>
+    <col min="4" max="4" width="46.28515625" customWidth="1"/>
+    <col min="5" max="5" width="32.28515625" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="19.6640625" customWidth="1"/>
-    <col min="8" max="8" width="16.109375" customWidth="1"/>
-    <col min="9" max="9" width="34.88671875" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" customWidth="1"/>
+    <col min="9" max="9" width="34.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -714,7 +795,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -743,7 +824,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="82.8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>18</v>
       </c>
@@ -772,7 +853,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>23</v>
       </c>
@@ -801,7 +882,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="57" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>28</v>
       </c>
@@ -830,7 +911,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>32</v>
       </c>
@@ -857,7 +938,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="57" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>45</v>
       </c>
@@ -882,7 +963,7 @@
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
     </row>
-    <row r="8" spans="1:9" ht="69" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>44</v>
       </c>
@@ -907,14 +988,14 @@
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
     </row>
-    <row r="9" spans="1:9" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>46</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D9" s="5" t="s">
@@ -930,18 +1011,30 @@
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
     </row>
-    <row r="10" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
+    <row r="10" spans="1:9" ht="57.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>52</v>
+      </c>
       <c r="E10" s="5"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="5"/>
+      <c r="F10" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>51</v>
+      </c>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
     </row>
-    <row r="11" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -952,7 +1045,7 @@
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
     </row>
-    <row r="12" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -963,7 +1056,7 @@
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
     </row>
-    <row r="13" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -974,7 +1067,7 @@
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
     </row>
-    <row r="14" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -985,7 +1078,7 @@
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
     </row>
-    <row r="15" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -996,7 +1089,7 @@
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
     </row>
-    <row r="16" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -1009,6 +1102,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
SRS first review Answer SIQ opened questions Signed-off-by: MMohamedAli74 <mmohamedali74@gmail.com>
</commit_message>
<xml_diff>
--- a/Input documents/SIQ.xlsx
+++ b/Input documents/SIQ.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="56">
   <si>
     <t>Req ID</t>
   </si>
@@ -253,6 +253,9 @@
   </si>
   <si>
     <t>the second operand will be negative signed</t>
+  </si>
+  <si>
+    <t>it should not allow it if it is multiplication or division od addition but should allow it if it is just subtraction as it should mean a sign in such case.</t>
   </si>
 </sst>
 </file>
@@ -769,8 +772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75"/>
@@ -1013,7 +1016,7 @@
         <v>44014</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="71.25">
@@ -1063,7 +1066,9 @@
       <c r="G10" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="H10" s="8"/>
+      <c r="H10" s="7">
+        <v>44014</v>
+      </c>
       <c r="I10" s="1" t="s">
         <v>54</v>
       </c>

</xml_diff>